<commit_message>
Updating the discrete SL varimp
</commit_message>
<xml_diff>
--- a/Analysis/update_data/data/processed/Data_Dictionary.xlsx
+++ b/Analysis/update_data/data/processed/Data_Dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmccoy/Documents/PhD/covid/GetzHubbard/Analysis/update_data/data/processed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmccoy/Documents/PhD/covid/Covid_SL_intxns/Covid_SL_intxns/Analysis/update_data/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0450D84-D0F4-F445-B0F2-7FAD32FB6E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDDE62F-F824-644B-AED8-A381DBC76DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34720" yWindow="2100" windowWidth="28800" windowHeight="13580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31480" yWindow="3600" windowWidth="28800" windowHeight="13580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2417" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2750" uniqueCount="720">
   <si>
     <t>Col Num</t>
   </si>
@@ -2775,6 +2775,186 @@
   </si>
   <si>
     <t>decile</t>
+  </si>
+  <si>
+    <t>1,2,3-Trichloropropane</t>
+  </si>
+  <si>
+    <t>Chromium (hexavalent)</t>
+  </si>
+  <si>
+    <t>Perfluorinated chemicals</t>
+  </si>
+  <si>
+    <t>Total trihalomethanes (TTHMs)</t>
+  </si>
+  <si>
+    <t>1,4-Dioxane</t>
+  </si>
+  <si>
+    <t>Bromodichloromethane</t>
+  </si>
+  <si>
+    <t>Chloroform</t>
+  </si>
+  <si>
+    <t>Dichloroacetic acid</t>
+  </si>
+  <si>
+    <t>Trichloroacetic acid</t>
+  </si>
+  <si>
+    <t>Radiological contaminants</t>
+  </si>
+  <si>
+    <t>Manganese</t>
+  </si>
+  <si>
+    <t>Dibromochloromethane</t>
+  </si>
+  <si>
+    <t>Tetrachloroethylene (perchloroethylene)</t>
+  </si>
+  <si>
+    <t>Haloacetic acids (HAA5)</t>
+  </si>
+  <si>
+    <t>Hormones</t>
+  </si>
+  <si>
+    <t>Arsenic</t>
+  </si>
+  <si>
+    <t>Trichloroethylene</t>
+  </si>
+  <si>
+    <t>Atrazine</t>
+  </si>
+  <si>
+    <t>Chlorate</t>
+  </si>
+  <si>
+    <t>Thallium</t>
+  </si>
+  <si>
+    <t>Chlorite</t>
+  </si>
+  <si>
+    <t>Bromate</t>
+  </si>
+  <si>
+    <t>Bromoform</t>
+  </si>
+  <si>
+    <t>Nitrate</t>
+  </si>
+  <si>
+    <t>Benzo[a]pyrene</t>
+  </si>
+  <si>
+    <t>Nitrate and nitrite</t>
+  </si>
+  <si>
+    <t>Cadmium</t>
+  </si>
+  <si>
+    <t>Beryllium</t>
+  </si>
+  <si>
+    <t>Antimony</t>
+  </si>
+  <si>
+    <t>Strontium</t>
+  </si>
+  <si>
+    <t>Benzene</t>
+  </si>
+  <si>
+    <t>Mercury (inorganic)</t>
+  </si>
+  <si>
+    <t>Perchlorate</t>
+  </si>
+  <si>
+    <t>Carbon tetrachloride</t>
+  </si>
+  <si>
+    <t>Vinyl chloride</t>
+  </si>
+  <si>
+    <t>1,2-Dichloroethane</t>
+  </si>
+  <si>
+    <t>Barium</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Chloromethane</t>
+  </si>
+  <si>
+    <t>Heptachlor epoxide</t>
+  </si>
+  <si>
+    <t>Fluoride</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>1,1,2-Trichloroethane</t>
+  </si>
+  <si>
+    <t>Chlordane</t>
+  </si>
+  <si>
+    <t>Lindane</t>
+  </si>
+  <si>
+    <t>Heptachlor</t>
+  </si>
+  <si>
+    <t>1,2-Dichloropropane</t>
+  </si>
+  <si>
+    <t>Styrene</t>
+  </si>
+  <si>
+    <t>1,2-Dibromo-3-chloropropane (DBCP)</t>
+  </si>
+  <si>
+    <t>Ethylene dibromide</t>
+  </si>
+  <si>
+    <t>Molybdenum</t>
+  </si>
+  <si>
+    <t>Polychlorinated biphenyls (PCBs)</t>
+  </si>
+  <si>
+    <t>1,3-Butadiene</t>
+  </si>
+  <si>
+    <t>Di(2-ethylhexyl) phthalate</t>
+  </si>
+  <si>
+    <t>Carbofuran</t>
+  </si>
+  <si>
+    <t>p-Dichlorobenzene</t>
+  </si>
+  <si>
+    <t>Glyphosate</t>
+  </si>
+  <si>
+    <t>Vanadium</t>
+  </si>
+  <si>
+    <t>MTBE</t>
+  </si>
+  <si>
+    <t>N-Nitrosodimethylamine (NDMA)</t>
   </si>
 </sst>
 </file>
@@ -3435,10 +3615,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J359"/>
+  <dimension ref="A1:J419"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A338" zoomScale="89" workbookViewId="0">
-      <selection activeCell="B349" sqref="B349"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="89" workbookViewId="0">
+      <selection activeCell="A193" sqref="A193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.19921875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8786,7 +8966,7 @@
         <v>461</v>
       </c>
       <c r="I193" s="6" t="s">
-        <v>268</v>
+        <v>17</v>
       </c>
     </row>
     <row r="194" spans="2:9" ht="14" x14ac:dyDescent="0.15">
@@ -8803,7 +8983,7 @@
         <v>461</v>
       </c>
       <c r="I194" s="6" t="s">
-        <v>268</v>
+        <v>17</v>
       </c>
     </row>
     <row r="195" spans="2:9" ht="14" x14ac:dyDescent="0.15">
@@ -8820,7 +9000,7 @@
         <v>461</v>
       </c>
       <c r="I195" s="6" t="s">
-        <v>268</v>
+        <v>17</v>
       </c>
     </row>
     <row r="196" spans="2:9" ht="14" x14ac:dyDescent="0.15">
@@ -8837,7 +9017,7 @@
         <v>461</v>
       </c>
       <c r="I196" s="6" t="s">
-        <v>268</v>
+        <v>17</v>
       </c>
     </row>
     <row r="197" spans="2:9" ht="14" x14ac:dyDescent="0.15">
@@ -8854,7 +9034,7 @@
         <v>461</v>
       </c>
       <c r="I197" s="6" t="s">
-        <v>268</v>
+        <v>17</v>
       </c>
     </row>
     <row r="198" spans="2:9" ht="14" x14ac:dyDescent="0.15">
@@ -11392,6 +11572,846 @@
         <v>264</v>
       </c>
       <c r="I359" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="360" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B360" s="55" t="s">
+        <v>660</v>
+      </c>
+      <c r="E360" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F360" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I360" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="361" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B361" s="55" t="s">
+        <v>661</v>
+      </c>
+      <c r="E361" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F361" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I361" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="362" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B362" s="55" t="s">
+        <v>662</v>
+      </c>
+      <c r="E362" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F362" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I362" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="363" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B363" s="55" t="s">
+        <v>663</v>
+      </c>
+      <c r="E363" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F363" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I363" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="364" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B364" s="55" t="s">
+        <v>664</v>
+      </c>
+      <c r="E364" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F364" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I364" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="365" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B365" s="55" t="s">
+        <v>665</v>
+      </c>
+      <c r="E365" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F365" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I365" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="366" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B366" s="55" t="s">
+        <v>666</v>
+      </c>
+      <c r="E366" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F366" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I366" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="367" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B367" s="55" t="s">
+        <v>667</v>
+      </c>
+      <c r="E367" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F367" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I367" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="368" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B368" s="55" t="s">
+        <v>668</v>
+      </c>
+      <c r="E368" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F368" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I368" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="369" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B369" s="55" t="s">
+        <v>669</v>
+      </c>
+      <c r="E369" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F369" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I369" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="370" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B370" s="55" t="s">
+        <v>670</v>
+      </c>
+      <c r="E370" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F370" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I370" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="371" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B371" s="55" t="s">
+        <v>671</v>
+      </c>
+      <c r="E371" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F371" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I371" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="372" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B372" s="55" t="s">
+        <v>672</v>
+      </c>
+      <c r="E372" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F372" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I372" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="373" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B373" s="55" t="s">
+        <v>673</v>
+      </c>
+      <c r="E373" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F373" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I373" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="374" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B374" s="55" t="s">
+        <v>674</v>
+      </c>
+      <c r="E374" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F374" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I374" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="375" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B375" s="55" t="s">
+        <v>675</v>
+      </c>
+      <c r="E375" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F375" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I375" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="376" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B376" s="55" t="s">
+        <v>676</v>
+      </c>
+      <c r="E376" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F376" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I376" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="377" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B377" s="55" t="s">
+        <v>677</v>
+      </c>
+      <c r="E377" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F377" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I377" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="378" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B378" s="55" t="s">
+        <v>678</v>
+      </c>
+      <c r="E378" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F378" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I378" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="379" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B379" s="55" t="s">
+        <v>679</v>
+      </c>
+      <c r="E379" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F379" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I379" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="380" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B380" s="55" t="s">
+        <v>680</v>
+      </c>
+      <c r="E380" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F380" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I380" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="381" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B381" s="55" t="s">
+        <v>681</v>
+      </c>
+      <c r="E381" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F381" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I381" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="382" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B382" s="55" t="s">
+        <v>682</v>
+      </c>
+      <c r="E382" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F382" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I382" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="383" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B383" s="55" t="s">
+        <v>683</v>
+      </c>
+      <c r="E383" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F383" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I383" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="384" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B384" s="55" t="s">
+        <v>684</v>
+      </c>
+      <c r="E384" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F384" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I384" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="385" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B385" s="55" t="s">
+        <v>685</v>
+      </c>
+      <c r="E385" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F385" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I385" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="386" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B386" s="55" t="s">
+        <v>686</v>
+      </c>
+      <c r="E386" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F386" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I386" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="387" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B387" s="55" t="s">
+        <v>687</v>
+      </c>
+      <c r="E387" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F387" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I387" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="388" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B388" s="55" t="s">
+        <v>688</v>
+      </c>
+      <c r="E388" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F388" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I388" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="389" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B389" s="55" t="s">
+        <v>689</v>
+      </c>
+      <c r="E389" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F389" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I389" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="390" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B390" s="55" t="s">
+        <v>690</v>
+      </c>
+      <c r="E390" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F390" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I390" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="391" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B391" s="55" t="s">
+        <v>691</v>
+      </c>
+      <c r="E391" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F391" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I391" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="392" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B392" s="55" t="s">
+        <v>692</v>
+      </c>
+      <c r="E392" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F392" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I392" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="393" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B393" s="55" t="s">
+        <v>693</v>
+      </c>
+      <c r="E393" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F393" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I393" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="394" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B394" s="55" t="s">
+        <v>694</v>
+      </c>
+      <c r="E394" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F394" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I394" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="395" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B395" s="55" t="s">
+        <v>695</v>
+      </c>
+      <c r="E395" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F395" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I395" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="396" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B396" s="55" t="s">
+        <v>696</v>
+      </c>
+      <c r="E396" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F396" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I396" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="397" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B397" s="55" t="s">
+        <v>697</v>
+      </c>
+      <c r="E397" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F397" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I397" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="398" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B398" s="55" t="s">
+        <v>698</v>
+      </c>
+      <c r="E398" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F398" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I398" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="399" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B399" s="55" t="s">
+        <v>699</v>
+      </c>
+      <c r="E399" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F399" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I399" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="400" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B400" s="55" t="s">
+        <v>700</v>
+      </c>
+      <c r="E400" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F400" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I400" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="401" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B401" s="55" t="s">
+        <v>701</v>
+      </c>
+      <c r="E401" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F401" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I401" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="402" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B402" s="55" t="s">
+        <v>702</v>
+      </c>
+      <c r="E402" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F402" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I402" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="403" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B403" s="55" t="s">
+        <v>703</v>
+      </c>
+      <c r="E403" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F403" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I403" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="404" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B404" s="55" t="s">
+        <v>704</v>
+      </c>
+      <c r="E404" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F404" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I404" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="405" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B405" s="55" t="s">
+        <v>705</v>
+      </c>
+      <c r="E405" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F405" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I405" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="406" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B406" s="55" t="s">
+        <v>706</v>
+      </c>
+      <c r="E406" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F406" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I406" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="407" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B407" s="55" t="s">
+        <v>707</v>
+      </c>
+      <c r="E407" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F407" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I407" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="408" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B408" s="55" t="s">
+        <v>708</v>
+      </c>
+      <c r="E408" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F408" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I408" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="409" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B409" s="55" t="s">
+        <v>709</v>
+      </c>
+      <c r="E409" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F409" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I409" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="410" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B410" s="55" t="s">
+        <v>710</v>
+      </c>
+      <c r="E410" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F410" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I410" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="411" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B411" s="55" t="s">
+        <v>711</v>
+      </c>
+      <c r="E411" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F411" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I411" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="412" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B412" s="55" t="s">
+        <v>712</v>
+      </c>
+      <c r="E412" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F412" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I412" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="413" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B413" s="55" t="s">
+        <v>713</v>
+      </c>
+      <c r="E413" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F413" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I413" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="414" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B414" s="55" t="s">
+        <v>714</v>
+      </c>
+      <c r="E414" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F414" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I414" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="415" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B415" s="55" t="s">
+        <v>715</v>
+      </c>
+      <c r="E415" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F415" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I415" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="416" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B416" s="55" t="s">
+        <v>716</v>
+      </c>
+      <c r="E416" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F416" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I416" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="417" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B417" s="55" t="s">
+        <v>717</v>
+      </c>
+      <c r="E417" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F417" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I417" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="418" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B418" s="55" t="s">
+        <v>718</v>
+      </c>
+      <c r="E418" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F418" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I418" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="419" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="B419" s="55" t="s">
+        <v>719</v>
+      </c>
+      <c r="E419" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F419" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I419" s="6" t="s">
         <v>268</v>
       </c>
     </row>
@@ -12071,150 +13091,497 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A271BEB6-EA4F-BF4D-A000-7E236290F5CB}">
-  <dimension ref="H13:H39"/>
+  <dimension ref="F5:BM66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:H39"/>
+      <selection activeCell="F7" sqref="F7:F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="8" max="9" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H13" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="14" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H14" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="15" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H15" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="16" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H16" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H17" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H18" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H19" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H20" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H21" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H22" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H23" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H24" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H25" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H26" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H27" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H28" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H29" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H30" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H31" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H32" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H33" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H34" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H35" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H36" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H37" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H38" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.15">
-      <c r="H39" t="s">
-        <v>638</v>
+    <row r="5" spans="6:65" x14ac:dyDescent="0.15">
+      <c r="F5" s="55" t="s">
+        <v>660</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>661</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>662</v>
+      </c>
+      <c r="I5" s="55" t="s">
+        <v>663</v>
+      </c>
+      <c r="J5" s="55" t="s">
+        <v>664</v>
+      </c>
+      <c r="K5" s="55" t="s">
+        <v>665</v>
+      </c>
+      <c r="L5" s="55" t="s">
+        <v>666</v>
+      </c>
+      <c r="M5" s="55" t="s">
+        <v>667</v>
+      </c>
+      <c r="N5" s="55" t="s">
+        <v>668</v>
+      </c>
+      <c r="O5" s="55" t="s">
+        <v>669</v>
+      </c>
+      <c r="P5" s="55" t="s">
+        <v>670</v>
+      </c>
+      <c r="Q5" s="55" t="s">
+        <v>671</v>
+      </c>
+      <c r="R5" s="55" t="s">
+        <v>672</v>
+      </c>
+      <c r="S5" s="55" t="s">
+        <v>673</v>
+      </c>
+      <c r="T5" s="55" t="s">
+        <v>674</v>
+      </c>
+      <c r="U5" s="55" t="s">
+        <v>675</v>
+      </c>
+      <c r="V5" s="55" t="s">
+        <v>676</v>
+      </c>
+      <c r="W5" s="55" t="s">
+        <v>677</v>
+      </c>
+      <c r="X5" s="55" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y5" s="55" t="s">
+        <v>679</v>
+      </c>
+      <c r="Z5" s="55" t="s">
+        <v>680</v>
+      </c>
+      <c r="AA5" s="55" t="s">
+        <v>681</v>
+      </c>
+      <c r="AB5" s="55" t="s">
+        <v>682</v>
+      </c>
+      <c r="AC5" s="55" t="s">
+        <v>683</v>
+      </c>
+      <c r="AD5" s="55" t="s">
+        <v>684</v>
+      </c>
+      <c r="AE5" s="55" t="s">
+        <v>685</v>
+      </c>
+      <c r="AF5" s="55" t="s">
+        <v>686</v>
+      </c>
+      <c r="AG5" s="55" t="s">
+        <v>687</v>
+      </c>
+      <c r="AH5" s="55" t="s">
+        <v>688</v>
+      </c>
+      <c r="AI5" s="55" t="s">
+        <v>689</v>
+      </c>
+      <c r="AJ5" s="55" t="s">
+        <v>690</v>
+      </c>
+      <c r="AK5" s="55" t="s">
+        <v>691</v>
+      </c>
+      <c r="AL5" s="55" t="s">
+        <v>692</v>
+      </c>
+      <c r="AM5" s="55" t="s">
+        <v>693</v>
+      </c>
+      <c r="AN5" s="55" t="s">
+        <v>694</v>
+      </c>
+      <c r="AO5" s="55" t="s">
+        <v>695</v>
+      </c>
+      <c r="AP5" s="55" t="s">
+        <v>696</v>
+      </c>
+      <c r="AQ5" s="55" t="s">
+        <v>697</v>
+      </c>
+      <c r="AR5" s="55" t="s">
+        <v>698</v>
+      </c>
+      <c r="AS5" s="55" t="s">
+        <v>699</v>
+      </c>
+      <c r="AT5" s="55" t="s">
+        <v>700</v>
+      </c>
+      <c r="AU5" s="55" t="s">
+        <v>701</v>
+      </c>
+      <c r="AV5" s="55" t="s">
+        <v>702</v>
+      </c>
+      <c r="AW5" s="55" t="s">
+        <v>703</v>
+      </c>
+      <c r="AX5" s="55" t="s">
+        <v>704</v>
+      </c>
+      <c r="AY5" s="55" t="s">
+        <v>705</v>
+      </c>
+      <c r="AZ5" s="55" t="s">
+        <v>706</v>
+      </c>
+      <c r="BA5" s="55" t="s">
+        <v>707</v>
+      </c>
+      <c r="BB5" s="55" t="s">
+        <v>708</v>
+      </c>
+      <c r="BC5" s="55" t="s">
+        <v>709</v>
+      </c>
+      <c r="BD5" s="55" t="s">
+        <v>710</v>
+      </c>
+      <c r="BE5" s="55" t="s">
+        <v>711</v>
+      </c>
+      <c r="BF5" s="55" t="s">
+        <v>712</v>
+      </c>
+      <c r="BG5" s="55" t="s">
+        <v>713</v>
+      </c>
+      <c r="BH5" s="55" t="s">
+        <v>714</v>
+      </c>
+      <c r="BI5" s="55" t="s">
+        <v>715</v>
+      </c>
+      <c r="BJ5" s="55" t="s">
+        <v>716</v>
+      </c>
+      <c r="BK5" s="55" t="s">
+        <v>717</v>
+      </c>
+      <c r="BL5" s="55" t="s">
+        <v>718</v>
+      </c>
+      <c r="BM5" s="55" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="7" spans="6:65" x14ac:dyDescent="0.15">
+      <c r="F7" s="55" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="8" spans="6:65" x14ac:dyDescent="0.15">
+      <c r="F8" s="55" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="9" spans="6:65" x14ac:dyDescent="0.15">
+      <c r="F9" s="55" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="10" spans="6:65" x14ac:dyDescent="0.15">
+      <c r="F10" s="55" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="11" spans="6:65" x14ac:dyDescent="0.15">
+      <c r="F11" s="55" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="12" spans="6:65" x14ac:dyDescent="0.15">
+      <c r="F12" s="55" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="13" spans="6:65" x14ac:dyDescent="0.15">
+      <c r="F13" s="55" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="14" spans="6:65" x14ac:dyDescent="0.15">
+      <c r="F14" s="55" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="15" spans="6:65" x14ac:dyDescent="0.15">
+      <c r="F15" s="55" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="16" spans="6:65" x14ac:dyDescent="0.15">
+      <c r="F16" s="55" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F17" s="55" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F18" s="55" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F19" s="55" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F20" s="55" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F21" s="55" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F22" s="55" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F23" s="55" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F24" s="55" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F25" s="55" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F26" s="55" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F27" s="55" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F28" s="55" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F29" s="55" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F30" s="55" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F31" s="55" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F32" s="55" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F33" s="55" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F34" s="55" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F35" s="55" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F36" s="55" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F37" s="55" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F38" s="55" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F39" s="55" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F40" s="55" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F41" s="55" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F42" s="55" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F43" s="55" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F44" s="55" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F45" s="55" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F46" s="55" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F47" s="55" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F48" s="55" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F49" s="55" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F50" s="55" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F51" s="55" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F52" s="55" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F53" s="55" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F54" s="55" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F55" s="55" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F56" s="55" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F57" s="55" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F58" s="55" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F59" s="55" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F60" s="55" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F61" s="55" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F62" s="55" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F63" s="55" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F64" s="55" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F65" s="55" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F66" s="55" t="s">
+        <v>719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish combining the preprocessing and spot checked the data
</commit_message>
<xml_diff>
--- a/Analysis/update_data/data/processed/Data_Dictionary.xlsx
+++ b/Analysis/update_data/data/processed/Data_Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunwenji/Downloads/Covid_SL_intxns/Analysis/update_data/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C17B7F-D025-6240-8703-27A25EC3576E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184AB013-DC8F-4044-A053-838FBEAF042F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19400" yWindow="0" windowWidth="19000" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10040" yWindow="460" windowWidth="19000" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3100" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3100" uniqueCount="925">
   <si>
     <t>Col Num</t>
   </si>
@@ -2507,18 +2507,6 @@
     <t>total_jail_pretrial_rate</t>
   </si>
   <si>
-    <t>black_white_jail_pop_rate</t>
-  </si>
-  <si>
-    <t>aapi_white_jail_pop_rate</t>
-  </si>
-  <si>
-    <t>latinx_white_jail_pop_rate</t>
-  </si>
-  <si>
-    <t>native_white_jail_pop_rate</t>
-  </si>
-  <si>
     <t>white_pop_15to64_ratio</t>
   </si>
   <si>
@@ -3479,39 +3467,12 @@
     <t>Lead Risk Decile</t>
   </si>
   <si>
-    <t>Nitrate.and.nitrite</t>
-  </si>
-  <si>
     <t>Comp 2,4-D</t>
   </si>
   <si>
     <t>Comp 2,4-DB</t>
   </si>
   <si>
-    <t>Trichloroacetic.acid</t>
-  </si>
-  <si>
-    <t>Radiological.contaminants</t>
-  </si>
-  <si>
-    <t>Tetrachloroethylene..perchloroethylene.</t>
-  </si>
-  <si>
-    <t>Dichloroacetic.acid</t>
-  </si>
-  <si>
-    <t>Chromium..hexavalent.</t>
-  </si>
-  <si>
-    <t>Haloacetic.acids..HAA5.</t>
-  </si>
-  <si>
-    <t>Total.trihalomethanes..TTHMs.</t>
-  </si>
-  <si>
-    <t>Perfluorinated.chemicals</t>
-  </si>
-  <si>
     <t>Hispanic White College Ratio</t>
   </si>
   <si>
@@ -3597,6 +3558,18 @@
   </si>
   <si>
     <t>avg_PCE_levels</t>
+  </si>
+  <si>
+    <t>white_black_jail_pop_rate</t>
+  </si>
+  <si>
+    <t>white_aapi_jail_pop_rate</t>
+  </si>
+  <si>
+    <t>white_latinx_jail_pop_rate</t>
+  </si>
+  <si>
+    <t>white_native_jail_pop_rate</t>
   </si>
 </sst>
 </file>
@@ -4302,8 +4275,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K419"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B281" sqref="B281"/>
+    <sheetView tabSelected="1" topLeftCell="A344" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B385" sqref="B385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.19921875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4325,7 +4298,7 @@
         <v>383</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>1</v>
@@ -4457,7 +4430,7 @@
         <v>178</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>4</v>
@@ -4522,7 +4495,7 @@
         <v>183</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>4</v>
@@ -4554,7 +4527,7 @@
         <v>385</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>4</v>
@@ -4586,7 +4559,7 @@
         <v>187</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>4</v>
@@ -4618,7 +4591,7 @@
         <v>189</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>4</v>
@@ -4650,7 +4623,7 @@
         <v>191</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>4</v>
@@ -4682,7 +4655,7 @@
         <v>193</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>4</v>
@@ -4714,7 +4687,7 @@
         <v>195</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>4</v>
@@ -4746,7 +4719,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>4</v>
@@ -4778,7 +4751,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>4</v>
@@ -4810,7 +4783,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>4</v>
@@ -4842,7 +4815,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>4</v>
@@ -4874,7 +4847,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>4</v>
@@ -4906,7 +4879,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>4</v>
@@ -4938,7 +4911,7 @@
         <v>42</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>4</v>
@@ -4970,7 +4943,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>4</v>
@@ -5035,7 +5008,7 @@
         <v>50</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>4</v>
@@ -5067,7 +5040,7 @@
         <v>386</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>4</v>
@@ -5168,7 +5141,7 @@
         <v>387</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>4</v>
@@ -5200,7 +5173,7 @@
         <v>388</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>4</v>
@@ -5232,7 +5205,7 @@
         <v>389</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>4</v>
@@ -5297,7 +5270,7 @@
         <v>390</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>4</v>
@@ -5329,7 +5302,7 @@
         <v>391</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>4</v>
@@ -5359,7 +5332,7 @@
         <v>408</v>
       </c>
       <c r="C33" s="57" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -5383,7 +5356,7 @@
         <v>392</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>4</v>
@@ -5415,7 +5388,7 @@
         <v>393</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>4</v>
@@ -5450,7 +5423,7 @@
         <v>394</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>4</v>
@@ -5515,7 +5488,7 @@
         <v>52</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>906</v>
+        <v>893</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
@@ -5548,10 +5521,10 @@
         <v>53</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>907</v>
+        <v>894</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>4</v>
@@ -5583,7 +5556,7 @@
         <v>103</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>4</v>
@@ -5615,7 +5588,7 @@
         <v>105</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>4</v>
@@ -5644,7 +5617,7 @@
         <v>56</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>908</v>
+        <v>895</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
@@ -5680,7 +5653,7 @@
         <v>108</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>4</v>
@@ -5709,10 +5682,10 @@
         <v>58</v>
       </c>
       <c r="B44" s="55" t="s">
-        <v>909</v>
+        <v>896</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>4</v>
@@ -5744,7 +5717,7 @@
         <v>111</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>4</v>
@@ -5776,7 +5749,7 @@
         <v>113</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>4</v>
@@ -5808,7 +5781,7 @@
         <v>115</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>4</v>
@@ -5837,10 +5810,10 @@
         <v>62</v>
       </c>
       <c r="B48" s="55" t="s">
-        <v>910</v>
+        <v>897</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>4</v>
@@ -5869,7 +5842,7 @@
         <v>63</v>
       </c>
       <c r="B49" s="55" t="s">
-        <v>911</v>
+        <v>898</v>
       </c>
       <c r="C49" s="55"/>
       <c r="D49" s="2" t="s">
@@ -5905,7 +5878,7 @@
         <v>119</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>4</v>
@@ -5935,10 +5908,10 @@
     <row r="51" spans="1:11" ht="28" x14ac:dyDescent="0.15">
       <c r="A51" s="7"/>
       <c r="B51" s="2" t="s">
-        <v>912</v>
+        <v>899</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>4</v>
@@ -5968,7 +5941,7 @@
         <v>121</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>4</v>
@@ -5997,10 +5970,10 @@
         <v>66</v>
       </c>
       <c r="B53" s="55" t="s">
-        <v>913</v>
+        <v>900</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>4</v>
@@ -6032,7 +6005,7 @@
         <v>124</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>4</v>
@@ -6061,10 +6034,10 @@
         <v>68</v>
       </c>
       <c r="B55" s="55" t="s">
-        <v>914</v>
+        <v>901</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>4</v>
@@ -6126,7 +6099,7 @@
         <v>70</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>915</v>
+        <v>902</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
@@ -6222,7 +6195,7 @@
         <v>73</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>916</v>
+        <v>903</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
@@ -6342,7 +6315,7 @@
         <v>77</v>
       </c>
       <c r="B64" s="55" t="s">
-        <v>917</v>
+        <v>904</v>
       </c>
       <c r="C64" s="55"/>
       <c r="D64" s="4" t="s">
@@ -6372,7 +6345,7 @@
         <v>78</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>918</v>
+        <v>905</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
@@ -6462,7 +6435,7 @@
         <v>81</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>919</v>
+        <v>906</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
@@ -6492,7 +6465,7 @@
         <v>82</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>920</v>
+        <v>907</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4" t="s">
@@ -6522,7 +6495,7 @@
         <v>83</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>921</v>
+        <v>908</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
@@ -6612,7 +6585,7 @@
         <v>86</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>922</v>
+        <v>909</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
@@ -6732,7 +6705,7 @@
         <v>90</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>923</v>
+        <v>910</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="4" t="s">
@@ -6762,7 +6735,7 @@
         <v>91</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>924</v>
+        <v>911</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
@@ -6852,7 +6825,7 @@
         <v>94</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>925</v>
+        <v>912</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
@@ -6882,7 +6855,7 @@
         <v>95</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>926</v>
+        <v>913</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="4" t="s">
@@ -6915,7 +6888,7 @@
         <v>52</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>4</v>
@@ -6947,7 +6920,7 @@
         <v>395</v>
       </c>
       <c r="C84" s="58" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>4</v>
@@ -6979,7 +6952,7 @@
         <v>396</v>
       </c>
       <c r="C85" s="58" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>4</v>
@@ -7044,7 +7017,7 @@
         <v>403</v>
       </c>
       <c r="C87" s="58" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>4</v>
@@ -7076,7 +7049,7 @@
         <v>398</v>
       </c>
       <c r="C88" s="58" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>4</v>
@@ -7141,7 +7114,7 @@
         <v>397</v>
       </c>
       <c r="C90" s="58" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>4</v>
@@ -7296,7 +7269,7 @@
         <v>219</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>4</v>
@@ -7356,10 +7329,10 @@
         <v>7</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>21</v>
@@ -7386,10 +7359,10 @@
         <v>1</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>4</v>
@@ -7419,7 +7392,7 @@
         <v>409</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>4</v>
@@ -7446,10 +7419,10 @@
         <v>3</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>4</v>
@@ -7479,7 +7452,7 @@
         <v>11</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>4</v>
@@ -7509,7 +7482,7 @@
         <v>13</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>4</v>
@@ -7567,10 +7540,10 @@
     <row r="104" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="9"/>
       <c r="B104" s="4" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>4</v>
@@ -7593,10 +7566,10 @@
     <row r="105" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A105" s="9"/>
       <c r="B105" s="4" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>4</v>
@@ -7624,7 +7597,7 @@
         <v>55</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>4</v>
@@ -7656,7 +7629,7 @@
         <v>400</v>
       </c>
       <c r="C107" s="58" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>4</v>
@@ -7688,7 +7661,7 @@
         <v>401</v>
       </c>
       <c r="C108" s="58" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>4</v>
@@ -7817,7 +7790,7 @@
         <v>549</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>4</v>
@@ -7847,7 +7820,7 @@
         <v>550</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>4</v>
@@ -7877,7 +7850,7 @@
         <v>551</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>4</v>
@@ -7907,7 +7880,7 @@
         <v>552</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="D115" s="4" t="s">
         <v>4</v>
@@ -7937,7 +7910,7 @@
         <v>553</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="D116" s="4" t="s">
         <v>4</v>
@@ -7966,10 +7939,10 @@
         <v>130</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="D117" s="4" t="s">
         <v>4</v>
@@ -8091,7 +8064,7 @@
         <v>404</v>
       </c>
       <c r="C121" s="58" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>4</v>
@@ -8123,7 +8096,7 @@
         <v>402</v>
       </c>
       <c r="C122" s="58" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>4</v>
@@ -8155,7 +8128,7 @@
         <v>405</v>
       </c>
       <c r="C123" s="58" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>4</v>
@@ -8187,7 +8160,7 @@
         <v>406</v>
       </c>
       <c r="C124" s="58" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>4</v>
@@ -8219,7 +8192,7 @@
         <v>407</v>
       </c>
       <c r="C125" s="58" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>4</v>
@@ -8333,7 +8306,7 @@
         <v>298</v>
       </c>
       <c r="C129" s="17" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="D129" s="14"/>
       <c r="E129" s="14"/>
@@ -8419,7 +8392,7 @@
         <v>304</v>
       </c>
       <c r="C132" s="31" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D132" s="28"/>
       <c r="E132" s="28"/>
@@ -8448,7 +8421,7 @@
         <v>305</v>
       </c>
       <c r="C133" s="31" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="D133" s="28"/>
       <c r="E133" s="28"/>
@@ -8474,7 +8447,7 @@
         <v>306</v>
       </c>
       <c r="C134" s="31" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="D134" s="28"/>
       <c r="E134" s="28"/>
@@ -8500,7 +8473,7 @@
         <v>307</v>
       </c>
       <c r="C135" s="31" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="D135" s="28"/>
       <c r="E135" s="28"/>
@@ -8554,7 +8527,7 @@
         <v>313</v>
       </c>
       <c r="C137" s="40" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="D137" s="37"/>
       <c r="E137" s="37"/>
@@ -8583,7 +8556,7 @@
         <v>315</v>
       </c>
       <c r="C138" s="40" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="D138" s="37"/>
       <c r="E138" s="37"/>
@@ -8637,7 +8610,7 @@
         <v>318</v>
       </c>
       <c r="C140" s="26" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="D140" s="23"/>
       <c r="E140" s="23"/>
@@ -8666,7 +8639,7 @@
         <v>321</v>
       </c>
       <c r="C141" s="26" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="D141" s="23"/>
       <c r="E141" s="23"/>
@@ -8719,7 +8692,7 @@
         <v>324</v>
       </c>
       <c r="C143" s="26" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D143" s="23"/>
       <c r="E143" s="23"/>
@@ -8748,7 +8721,7 @@
         <v>326</v>
       </c>
       <c r="C144" s="26" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="D144" s="23"/>
       <c r="E144" s="23"/>
@@ -8779,7 +8752,7 @@
         <v>201</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="D145" s="4" t="s">
         <v>4</v>
@@ -8937,7 +8910,7 @@
         <v>224</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="D150" s="4" t="s">
         <v>4</v>
@@ -8972,7 +8945,7 @@
         <v>227</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D151" s="4" t="s">
         <v>4</v>
@@ -9037,7 +9010,7 @@
         <v>411</v>
       </c>
       <c r="C153" s="59" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>4</v>
@@ -9099,7 +9072,7 @@
         <v>198</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="D155" s="4" t="s">
         <v>4</v>
@@ -9131,7 +9104,7 @@
         <v>231</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="D156" s="4" t="s">
         <v>4</v>
@@ -9216,7 +9189,7 @@
         <v>366</v>
       </c>
       <c r="C159" s="50" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="D159" s="49"/>
       <c r="E159" s="49"/>
@@ -9242,7 +9215,7 @@
         <v>367</v>
       </c>
       <c r="C160" s="50" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="D160" s="49"/>
       <c r="E160" s="49"/>
@@ -9268,7 +9241,7 @@
         <v>368</v>
       </c>
       <c r="C161" s="50" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="D161" s="49"/>
       <c r="E161" s="49"/>
@@ -9294,7 +9267,7 @@
         <v>378</v>
       </c>
       <c r="C162" s="50" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D162" s="49"/>
       <c r="E162" s="49"/>
@@ -9320,7 +9293,7 @@
         <v>379</v>
       </c>
       <c r="C163" s="50" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D163" s="49"/>
       <c r="E163" s="49"/>
@@ -9346,7 +9319,7 @@
         <v>380</v>
       </c>
       <c r="C164" s="51" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="D164" s="49"/>
       <c r="E164" s="49"/>
@@ -9372,7 +9345,7 @@
         <v>381</v>
       </c>
       <c r="C165" s="51" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="D165" s="49"/>
       <c r="E165" s="49"/>
@@ -9398,7 +9371,7 @@
         <v>382</v>
       </c>
       <c r="C166" s="51" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="D166" s="49"/>
       <c r="E166" s="49"/>
@@ -9424,7 +9397,7 @@
         <v>377</v>
       </c>
       <c r="C167" s="51" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D167" s="49"/>
       <c r="E167" s="49"/>
@@ -9450,7 +9423,7 @@
         <v>376</v>
       </c>
       <c r="C168" s="51" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="D168" s="49"/>
       <c r="E168" s="49"/>
@@ -9476,7 +9449,7 @@
         <v>375</v>
       </c>
       <c r="C169" s="51" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="D169" s="49"/>
       <c r="E169" s="49"/>
@@ -9502,7 +9475,7 @@
         <v>374</v>
       </c>
       <c r="C170" s="51" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="D170" s="49"/>
       <c r="E170" s="49"/>
@@ -9528,7 +9501,7 @@
         <v>373</v>
       </c>
       <c r="C171" s="51" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D171" s="49"/>
       <c r="E171" s="49"/>
@@ -9554,7 +9527,7 @@
         <v>372</v>
       </c>
       <c r="C172" s="51" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="D172" s="49"/>
       <c r="E172" s="49"/>
@@ -9580,7 +9553,7 @@
         <v>371</v>
       </c>
       <c r="C173" s="51" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="D173" s="49"/>
       <c r="E173" s="49"/>
@@ -9606,7 +9579,7 @@
         <v>370</v>
       </c>
       <c r="C174" s="51" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D174" s="49"/>
       <c r="E174" s="49"/>
@@ -9632,7 +9605,7 @@
         <v>369</v>
       </c>
       <c r="C175" s="51" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D175" s="49"/>
       <c r="E175" s="49"/>
@@ -9657,7 +9630,7 @@
         <v>357</v>
       </c>
       <c r="C176" s="52" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="F176" s="52" t="s">
         <v>359</v>
@@ -9683,7 +9656,7 @@
         <v>361</v>
       </c>
       <c r="C177" s="60" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="D177" s="6" t="s">
         <v>417</v>
@@ -9715,7 +9688,7 @@
         <v>412</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D178" s="6" t="s">
         <v>417</v>
@@ -9747,7 +9720,7 @@
         <v>410</v>
       </c>
       <c r="C179" s="60" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D179" s="6" t="s">
         <v>417</v>
@@ -9779,7 +9752,7 @@
         <v>415</v>
       </c>
       <c r="C180" s="60" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="D180" s="6" t="s">
         <v>417</v>
@@ -9808,7 +9781,7 @@
         <v>419</v>
       </c>
       <c r="C181" s="6" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="D181" s="6" t="s">
         <v>417</v>
@@ -9834,7 +9807,7 @@
         <v>420</v>
       </c>
       <c r="C182" s="6" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="D182" s="6" t="s">
         <v>417</v>
@@ -9860,7 +9833,7 @@
         <v>421</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="D183" s="6" t="s">
         <v>417</v>
@@ -9886,7 +9859,7 @@
         <v>422</v>
       </c>
       <c r="C184" s="6" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="D184" s="6" t="s">
         <v>417</v>
@@ -9912,7 +9885,7 @@
         <v>423</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="D185" s="6" t="s">
         <v>417</v>
@@ -9938,7 +9911,7 @@
         <v>424</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="D186" s="6" t="s">
         <v>417</v>
@@ -9964,7 +9937,7 @@
         <v>427</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="F187" s="3" t="s">
         <v>251</v>
@@ -9984,7 +9957,7 @@
         <v>428</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="F188" s="3" t="s">
         <v>251</v>
@@ -10004,7 +9977,7 @@
         <v>429</v>
       </c>
       <c r="C189" s="6" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="F189" s="3" t="s">
         <v>251</v>
@@ -10024,7 +9997,7 @@
         <v>430</v>
       </c>
       <c r="C190" s="6" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="F190" s="3" t="s">
         <v>251</v>
@@ -10044,7 +10017,7 @@
         <v>431</v>
       </c>
       <c r="C191" s="6" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="F191" s="3" t="s">
         <v>251</v>
@@ -10064,7 +10037,7 @@
         <v>432</v>
       </c>
       <c r="C192" s="6" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="F192" s="3" t="s">
         <v>251</v>
@@ -10504,7 +10477,7 @@
         <v>441</v>
       </c>
       <c r="C214" s="61" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
       <c r="F214" s="3" t="s">
         <v>251</v>
@@ -10844,7 +10817,7 @@
         <v>442</v>
       </c>
       <c r="C231" s="61" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
       <c r="F231" s="3" t="s">
         <v>251</v>
@@ -11821,10 +11794,10 @@
     </row>
     <row r="280" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B280" s="6" t="s">
-        <v>927</v>
+        <v>914</v>
       </c>
       <c r="C280" s="6" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="F280" s="3" t="s">
         <v>251</v>
@@ -11841,10 +11814,10 @@
     </row>
     <row r="281" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B281" s="6" t="s">
-        <v>933</v>
+        <v>920</v>
       </c>
       <c r="C281" s="6" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="F281" s="3" t="s">
         <v>251</v>
@@ -11861,10 +11834,10 @@
     </row>
     <row r="282" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B282" s="6" t="s">
-        <v>928</v>
+        <v>915</v>
       </c>
       <c r="C282" s="6" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="F282" s="3" t="s">
         <v>251</v>
@@ -11881,10 +11854,10 @@
     </row>
     <row r="283" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B283" s="6" t="s">
-        <v>929</v>
+        <v>916</v>
       </c>
       <c r="C283" s="6" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="F283" s="3" t="s">
         <v>251</v>
@@ -11901,10 +11874,10 @@
     </row>
     <row r="284" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B284" s="6" t="s">
-        <v>930</v>
+        <v>917</v>
       </c>
       <c r="C284" s="6" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="F284" s="3" t="s">
         <v>251</v>
@@ -11921,10 +11894,10 @@
     </row>
     <row r="285" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B285" s="6" t="s">
-        <v>931</v>
+        <v>918</v>
       </c>
       <c r="C285" s="6" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="F285" s="3" t="s">
         <v>251</v>
@@ -11941,10 +11914,10 @@
     </row>
     <row r="286" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B286" s="6" t="s">
-        <v>932</v>
+        <v>919</v>
       </c>
       <c r="C286" s="6" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="F286" s="3" t="s">
         <v>251</v>
@@ -11964,7 +11937,7 @@
         <v>526</v>
       </c>
       <c r="C287" s="6" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="F287" s="3" t="s">
         <v>251</v>
@@ -11984,7 +11957,7 @@
         <v>530</v>
       </c>
       <c r="C288" s="61" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="F288" s="6" t="s">
         <v>80</v>
@@ -12001,7 +11974,7 @@
         <v>532</v>
       </c>
       <c r="C289" s="61" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="F289" s="6" t="s">
         <v>80</v>
@@ -12018,7 +11991,7 @@
         <v>534</v>
       </c>
       <c r="C290" s="61" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="F290" s="6" t="s">
         <v>80</v>
@@ -12035,7 +12008,7 @@
         <v>536</v>
       </c>
       <c r="C291" s="61" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="F291" s="6" t="s">
         <v>80</v>
@@ -12052,7 +12025,7 @@
         <v>538</v>
       </c>
       <c r="C292" s="61" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="F292" s="6" t="s">
         <v>80</v>
@@ -12069,7 +12042,7 @@
         <v>540</v>
       </c>
       <c r="C293" s="61" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="F293" s="6" t="s">
         <v>80</v>
@@ -12086,7 +12059,7 @@
         <v>542</v>
       </c>
       <c r="C294" s="61" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="F294" s="6" t="s">
         <v>80</v>
@@ -12103,7 +12076,7 @@
         <v>544</v>
       </c>
       <c r="C295" s="61" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="F295" s="6" t="s">
         <v>80</v>
@@ -12120,7 +12093,7 @@
         <v>546</v>
       </c>
       <c r="C296" s="61" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="F296" s="6" t="s">
         <v>80</v>
@@ -12137,13 +12110,13 @@
         <v>561</v>
       </c>
       <c r="C297" s="6" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="F297" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G297" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J297" s="6" t="s">
         <v>255</v>
@@ -12154,13 +12127,13 @@
         <v>562</v>
       </c>
       <c r="C298" s="6" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="F298" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G298" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J298" s="6" t="s">
         <v>255</v>
@@ -12171,13 +12144,13 @@
         <v>563</v>
       </c>
       <c r="C299" s="6" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="F299" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G299" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J299" s="6" t="s">
         <v>255</v>
@@ -12188,13 +12161,13 @@
         <v>564</v>
       </c>
       <c r="C300" s="6" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="F300" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G300" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J300" s="6" t="s">
         <v>255</v>
@@ -12205,13 +12178,13 @@
         <v>565</v>
       </c>
       <c r="C301" s="6" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="F301" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G301" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J301" s="6" t="s">
         <v>255</v>
@@ -12222,13 +12195,13 @@
         <v>566</v>
       </c>
       <c r="C302" s="6" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="F302" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G302" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J302" s="6" t="s">
         <v>255</v>
@@ -12239,13 +12212,13 @@
         <v>567</v>
       </c>
       <c r="C303" s="6" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="F303" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G303" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J303" s="6" t="s">
         <v>255</v>
@@ -12256,13 +12229,13 @@
         <v>568</v>
       </c>
       <c r="C304" s="6" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="F304" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G304" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J304" s="6" t="s">
         <v>255</v>
@@ -12273,13 +12246,13 @@
         <v>569</v>
       </c>
       <c r="C305" s="6" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="F305" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G305" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J305" s="6" t="s">
         <v>255</v>
@@ -12287,16 +12260,16 @@
     </row>
     <row r="306" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B306" s="6" t="s">
-        <v>570</v>
+        <v>921</v>
       </c>
       <c r="C306" s="6" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="F306" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G306" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J306" s="6" t="s">
         <v>255</v>
@@ -12304,16 +12277,16 @@
     </row>
     <row r="307" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B307" s="6" t="s">
-        <v>571</v>
+        <v>922</v>
       </c>
       <c r="C307" s="6" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="F307" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G307" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J307" s="6" t="s">
         <v>255</v>
@@ -12321,16 +12294,16 @@
     </row>
     <row r="308" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B308" s="6" t="s">
-        <v>572</v>
+        <v>923</v>
       </c>
       <c r="C308" s="6" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="F308" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G308" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J308" s="6" t="s">
         <v>255</v>
@@ -12338,16 +12311,16 @@
     </row>
     <row r="309" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B309" s="6" t="s">
-        <v>573</v>
+        <v>924</v>
       </c>
       <c r="C309" s="6" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="F309" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G309" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J309" s="6" t="s">
         <v>255</v>
@@ -12355,16 +12328,16 @@
     </row>
     <row r="310" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B310" s="6" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C310" s="6" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="F310" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G310" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J310" s="6" t="s">
         <v>255</v>
@@ -12372,19 +12345,19 @@
     </row>
     <row r="311" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A311" s="6" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="B311" s="6" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C311" s="6" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="F311" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G311" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J311" s="6" t="s">
         <v>255</v>
@@ -12392,16 +12365,16 @@
     </row>
     <row r="312" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B312" s="6" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="C312" s="6" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="F312" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G312" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J312" s="6" t="s">
         <v>255</v>
@@ -12409,16 +12382,16 @@
     </row>
     <row r="313" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B313" s="6" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C313" s="6" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="F313" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G313" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J313" s="6" t="s">
         <v>255</v>
@@ -12426,16 +12399,16 @@
     </row>
     <row r="314" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B314" s="6" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C314" s="6" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="F314" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G314" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J314" s="6" t="s">
         <v>255</v>
@@ -12443,16 +12416,16 @@
     </row>
     <row r="315" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B315" s="6" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C315" s="6" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="F315" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G315" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J315" s="6" t="s">
         <v>255</v>
@@ -12460,16 +12433,16 @@
     </row>
     <row r="316" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B316" s="6" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C316" s="6" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="F316" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G316" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J316" s="6" t="s">
         <v>255</v>
@@ -12477,16 +12450,16 @@
     </row>
     <row r="317" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B317" s="6" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C317" s="6" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="F317" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G317" s="6" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J317" s="6" t="s">
         <v>255</v>
@@ -12494,16 +12467,16 @@
     </row>
     <row r="318" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B318" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C318" s="61" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="F318" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G318" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J318" s="6" t="s">
         <v>255</v>
@@ -12511,16 +12484,16 @@
     </row>
     <row r="319" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B319" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="C319" s="61" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="F319" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G319" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J319" s="6" t="s">
         <v>255</v>
@@ -12528,16 +12501,16 @@
     </row>
     <row r="320" spans="1:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B320" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C320" s="62" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="F320" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G320" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J320" s="6" t="s">
         <v>255</v>
@@ -12545,16 +12518,16 @@
     </row>
     <row r="321" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B321" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="C321" s="62" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="F321" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G321" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J321" s="6" t="s">
         <v>255</v>
@@ -12562,16 +12535,16 @@
     </row>
     <row r="322" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B322" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C322" s="62" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="F322" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G322" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J322" s="6" t="s">
         <v>255</v>
@@ -12579,16 +12552,16 @@
     </row>
     <row r="323" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B323" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C323" s="61" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="F323" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G323" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J323" s="6" t="s">
         <v>255</v>
@@ -12596,16 +12569,16 @@
     </row>
     <row r="324" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B324" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="C324" s="61" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="F324" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G324" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J324" s="6" t="s">
         <v>255</v>
@@ -12613,16 +12586,16 @@
     </row>
     <row r="325" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B325" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C325" s="62" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="F325" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G325" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J325" s="6" t="s">
         <v>255</v>
@@ -12630,16 +12603,16 @@
     </row>
     <row r="326" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B326" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C326" s="62" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="F326" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G326" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J326" s="6" t="s">
         <v>255</v>
@@ -12647,16 +12620,16 @@
     </row>
     <row r="327" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B327" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="C327" s="62" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="F327" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G327" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J327" s="6" t="s">
         <v>255</v>
@@ -12664,16 +12637,16 @@
     </row>
     <row r="328" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B328" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="C328" s="61" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="F328" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G328" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J328" s="6" t="s">
         <v>255</v>
@@ -12681,16 +12654,16 @@
     </row>
     <row r="329" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B329" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C329" s="61" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="F329" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G329" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J329" s="6" t="s">
         <v>255</v>
@@ -12698,16 +12671,16 @@
     </row>
     <row r="330" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B330" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C330" s="62" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="F330" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G330" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J330" s="6" t="s">
         <v>255</v>
@@ -12715,16 +12688,16 @@
     </row>
     <row r="331" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B331" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="C331" s="62" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="F331" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G331" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J331" s="6" t="s">
         <v>255</v>
@@ -12732,16 +12705,16 @@
     </row>
     <row r="332" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B332" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="C332" s="61" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="F332" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G332" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J332" s="6" t="s">
         <v>255</v>
@@ -12749,16 +12722,16 @@
     </row>
     <row r="333" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B333" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C333" s="61" t="s">
-        <v>905</v>
+        <v>892</v>
       </c>
       <c r="F333" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G333" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J333" s="6" t="s">
         <v>255</v>
@@ -12766,24 +12739,24 @@
     </row>
     <row r="334" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B334" s="61" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C334" s="61" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="335" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B335" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="C335" s="62" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="F335" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G335" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J335" s="6" t="s">
         <v>255</v>
@@ -12791,16 +12764,16 @@
     </row>
     <row r="336" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B336" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C336" s="62" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="F336" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G336" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J336" s="6" t="s">
         <v>255</v>
@@ -12808,16 +12781,16 @@
     </row>
     <row r="337" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B337" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C337" s="62" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="F337" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G337" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J337" s="6" t="s">
         <v>255</v>
@@ -12825,16 +12798,16 @@
     </row>
     <row r="338" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B338" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="C338" s="62" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="F338" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G338" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J338" s="6" t="s">
         <v>255</v>
@@ -12842,16 +12815,16 @@
     </row>
     <row r="339" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B339" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="C339" s="62" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="F339" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G339" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J339" s="6" t="s">
         <v>255</v>
@@ -12859,16 +12832,16 @@
     </row>
     <row r="340" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B340" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="C340" s="62" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="F340" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G340" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J340" s="6" t="s">
         <v>255</v>
@@ -12876,16 +12849,16 @@
     </row>
     <row r="341" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B341" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="C341" s="61" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="F341" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G341" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J341" s="6" t="s">
         <v>255</v>
@@ -12893,16 +12866,16 @@
     </row>
     <row r="342" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B342" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C342" s="61" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="F342" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G342" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J342" s="6" t="s">
         <v>255</v>
@@ -12910,16 +12883,16 @@
     </row>
     <row r="343" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B343" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C343" s="61" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="F343" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G343" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J343" s="6" t="s">
         <v>255</v>
@@ -12927,16 +12900,16 @@
     </row>
     <row r="344" spans="2:10" ht="16" x14ac:dyDescent="0.15">
       <c r="B344" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="C344" s="62" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="F344" s="6" t="s">
         <v>80</v>
       </c>
       <c r="G344" s="6" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="J344" s="6" t="s">
         <v>255</v>
@@ -12944,10 +12917,10 @@
     </row>
     <row r="345" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B345" s="6" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C345" s="6" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="F345" s="6" t="s">
         <v>80</v>
@@ -12961,10 +12934,10 @@
     </row>
     <row r="346" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B346" s="6" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="C346" s="6" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="F346" s="6" t="s">
         <v>80</v>
@@ -12978,10 +12951,10 @@
     </row>
     <row r="347" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B347" s="6" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="C347" s="6" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="F347" s="6" t="s">
         <v>80</v>
@@ -12995,10 +12968,10 @@
     </row>
     <row r="348" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B348" s="6" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C348" s="6" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="F348" s="6" t="s">
         <v>80</v>
@@ -13012,10 +12985,10 @@
     </row>
     <row r="349" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B349" s="6" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="C349" s="6" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="F349" s="6" t="s">
         <v>80</v>
@@ -13029,10 +13002,10 @@
     </row>
     <row r="350" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B350" s="6" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C350" s="6" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="F350" s="6" t="s">
         <v>80</v>
@@ -13046,10 +13019,10 @@
     </row>
     <row r="351" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B351" s="6" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C351" s="6" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="F351" s="6" t="s">
         <v>80</v>
@@ -13063,10 +13036,10 @@
     </row>
     <row r="352" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B352" s="6" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C352" s="6" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="F352" s="6" t="s">
         <v>80</v>
@@ -13080,10 +13053,10 @@
     </row>
     <row r="353" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B353" s="6" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="C353" s="6" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="F353" s="6" t="s">
         <v>80</v>
@@ -13097,10 +13070,10 @@
     </row>
     <row r="354" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B354" s="6" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="C354" s="6" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="F354" s="6" t="s">
         <v>80</v>
@@ -13114,10 +13087,10 @@
     </row>
     <row r="355" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B355" s="6" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C355" s="6" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="F355" s="6" t="s">
         <v>80</v>
@@ -13131,10 +13104,10 @@
     </row>
     <row r="356" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B356" s="6" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C356" s="6" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="F356" s="6" t="s">
         <v>80</v>
@@ -13148,10 +13121,10 @@
     </row>
     <row r="357" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B357" s="6" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="C357" s="6" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="F357" s="6" t="s">
         <v>80</v>
@@ -13165,10 +13138,10 @@
     </row>
     <row r="358" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B358" s="6" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="C358" s="6" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="F358" s="6" t="s">
         <v>80</v>
@@ -13182,10 +13155,10 @@
     </row>
     <row r="359" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B359" s="6" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="C359" s="6" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
       <c r="F359" s="6" t="s">
         <v>80</v>
@@ -13199,16 +13172,16 @@
     </row>
     <row r="360" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B360" s="55" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="C360" s="55" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="F360" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G360" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J360" s="6" t="s">
         <v>255</v>
@@ -13216,16 +13189,16 @@
     </row>
     <row r="361" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B361" s="63" t="s">
-        <v>901</v>
+        <v>629</v>
       </c>
       <c r="C361" s="55" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="F361" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G361" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J361" s="6" t="s">
         <v>255</v>
@@ -13233,16 +13206,16 @@
     </row>
     <row r="362" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B362" s="63" t="s">
-        <v>904</v>
+        <v>630</v>
       </c>
       <c r="C362" s="55" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="F362" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G362" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J362" s="6" t="s">
         <v>255</v>
@@ -13250,16 +13223,16 @@
     </row>
     <row r="363" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B363" s="63" t="s">
-        <v>903</v>
+        <v>631</v>
       </c>
       <c r="C363" s="55" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="F363" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G363" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J363" s="6" t="s">
         <v>255</v>
@@ -13267,16 +13240,16 @@
     </row>
     <row r="364" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B364" s="55" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="C364" s="55" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="F364" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G364" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J364" s="6" t="s">
         <v>255</v>
@@ -13284,16 +13257,16 @@
     </row>
     <row r="365" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B365" s="55" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C365" s="55" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F365" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G365" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J365" s="6" t="s">
         <v>255</v>
@@ -13301,16 +13274,16 @@
     </row>
     <row r="366" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B366" s="55" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C366" s="55" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="F366" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G366" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J366" s="6" t="s">
         <v>255</v>
@@ -13318,16 +13291,16 @@
     </row>
     <row r="367" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B367" s="63" t="s">
-        <v>900</v>
+        <v>635</v>
       </c>
       <c r="C367" s="55" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="F367" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G367" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J367" s="6" t="s">
         <v>255</v>
@@ -13335,16 +13308,16 @@
     </row>
     <row r="368" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B368" s="63" t="s">
-        <v>897</v>
+        <v>636</v>
       </c>
       <c r="C368" s="55" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="F368" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G368" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J368" s="6" t="s">
         <v>255</v>
@@ -13352,16 +13325,16 @@
     </row>
     <row r="369" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B369" s="63" t="s">
-        <v>898</v>
+        <v>637</v>
       </c>
       <c r="C369" s="55" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="F369" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G369" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J369" s="6" t="s">
         <v>255</v>
@@ -13369,16 +13342,16 @@
     </row>
     <row r="370" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B370" s="55" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C370" s="55" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="F370" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G370" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J370" s="6" t="s">
         <v>255</v>
@@ -13386,16 +13359,16 @@
     </row>
     <row r="371" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B371" s="55" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C371" s="55" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="F371" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G371" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J371" s="6" t="s">
         <v>255</v>
@@ -13403,16 +13376,16 @@
     </row>
     <row r="372" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B372" s="63" t="s">
-        <v>899</v>
+        <v>640</v>
       </c>
       <c r="C372" s="55" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="F372" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G372" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J372" s="6" t="s">
         <v>255</v>
@@ -13420,16 +13393,16 @@
     </row>
     <row r="373" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B373" s="63" t="s">
-        <v>902</v>
+        <v>641</v>
       </c>
       <c r="C373" s="55" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="F373" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G373" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J373" s="6" t="s">
         <v>255</v>
@@ -13437,16 +13410,16 @@
     </row>
     <row r="374" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B374" s="55" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C374" s="55" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="F374" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G374" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J374" s="6" t="s">
         <v>255</v>
@@ -13454,16 +13427,16 @@
     </row>
     <row r="375" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B375" s="55" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C375" s="55" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="F375" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G375" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J375" s="6" t="s">
         <v>255</v>
@@ -13471,16 +13444,16 @@
     </row>
     <row r="376" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B376" s="55" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="C376" s="55" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="F376" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G376" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J376" s="6" t="s">
         <v>255</v>
@@ -13488,16 +13461,16 @@
     </row>
     <row r="377" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B377" s="55" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C377" s="55" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="F377" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G377" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J377" s="6" t="s">
         <v>255</v>
@@ -13505,16 +13478,16 @@
     </row>
     <row r="378" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B378" s="55" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C378" s="55" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="F378" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G378" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J378" s="6" t="s">
         <v>255</v>
@@ -13522,16 +13495,16 @@
     </row>
     <row r="379" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B379" s="55" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C379" s="55" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="F379" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G379" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J379" s="6" t="s">
         <v>255</v>
@@ -13539,16 +13512,16 @@
     </row>
     <row r="380" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B380" s="55" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="C380" s="55" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="F380" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G380" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J380" s="6" t="s">
         <v>255</v>
@@ -13556,16 +13529,16 @@
     </row>
     <row r="381" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B381" s="55" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C381" s="55" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="F381" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G381" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J381" s="6" t="s">
         <v>255</v>
@@ -13573,16 +13546,16 @@
     </row>
     <row r="382" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B382" s="55" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C382" s="55" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="F382" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G382" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J382" s="6" t="s">
         <v>255</v>
@@ -13590,16 +13563,16 @@
     </row>
     <row r="383" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B383" s="55" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C383" s="55" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="F383" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G383" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J383" s="6" t="s">
         <v>255</v>
@@ -13607,16 +13580,16 @@
     </row>
     <row r="384" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B384" s="55" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C384" s="55" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="F384" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G384" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J384" s="6" t="s">
         <v>255</v>
@@ -13624,16 +13597,16 @@
     </row>
     <row r="385" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B385" s="63" t="s">
-        <v>894</v>
+        <v>653</v>
       </c>
       <c r="C385" s="55" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="F385" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G385" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J385" s="6" t="s">
         <v>255</v>
@@ -13641,16 +13614,16 @@
     </row>
     <row r="386" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B386" s="55" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C386" s="55" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="F386" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G386" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J386" s="6" t="s">
         <v>255</v>
@@ -13658,16 +13631,16 @@
     </row>
     <row r="387" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B387" s="55" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C387" s="55" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="F387" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G387" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J387" s="6" t="s">
         <v>255</v>
@@ -13675,16 +13648,16 @@
     </row>
     <row r="388" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B388" s="55" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="C388" s="55" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="F388" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G388" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J388" s="6" t="s">
         <v>255</v>
@@ -13692,16 +13665,16 @@
     </row>
     <row r="389" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B389" s="55" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="C389" s="55" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="F389" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G389" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J389" s="6" t="s">
         <v>255</v>
@@ -13709,16 +13682,16 @@
     </row>
     <row r="390" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B390" s="55" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C390" s="55" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F390" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G390" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J390" s="6" t="s">
         <v>255</v>
@@ -13726,16 +13699,16 @@
     </row>
     <row r="391" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B391" s="55" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C391" s="55" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="F391" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G391" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J391" s="6" t="s">
         <v>255</v>
@@ -13743,16 +13716,16 @@
     </row>
     <row r="392" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B392" s="55" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C392" s="55" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="F392" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G392" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J392" s="6" t="s">
         <v>255</v>
@@ -13760,16 +13733,16 @@
     </row>
     <row r="393" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B393" s="55" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C393" s="55" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="F393" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G393" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J393" s="6" t="s">
         <v>255</v>
@@ -13777,16 +13750,16 @@
     </row>
     <row r="394" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B394" s="55" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C394" s="55" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="F394" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G394" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J394" s="6" t="s">
         <v>255</v>
@@ -13794,16 +13767,16 @@
     </row>
     <row r="395" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B395" s="55" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="C395" s="55" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="F395" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G395" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J395" s="6" t="s">
         <v>255</v>
@@ -13811,16 +13784,16 @@
     </row>
     <row r="396" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B396" s="55" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C396" s="55" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="F396" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G396" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J396" s="6" t="s">
         <v>255</v>
@@ -13828,16 +13801,16 @@
     </row>
     <row r="397" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B397" s="55" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C397" s="55" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="F397" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G397" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J397" s="6" t="s">
         <v>255</v>
@@ -13845,16 +13818,16 @@
     </row>
     <row r="398" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B398" s="55" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C398" s="55" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="F398" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G398" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J398" s="6" t="s">
         <v>255</v>
@@ -13862,16 +13835,16 @@
     </row>
     <row r="399" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B399" s="55" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C399" s="55" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="F399" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G399" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J399" s="6" t="s">
         <v>255</v>
@@ -13879,16 +13852,16 @@
     </row>
     <row r="400" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B400" s="55" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="C400" s="55" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="F400" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G400" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J400" s="6" t="s">
         <v>255</v>
@@ -13896,16 +13869,16 @@
     </row>
     <row r="401" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B401" s="55" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="C401" s="55" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="F401" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G401" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J401" s="6" t="s">
         <v>255</v>
@@ -13913,16 +13886,16 @@
     </row>
     <row r="402" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B402" s="55" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C402" s="55" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="F402" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G402" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J402" s="6" t="s">
         <v>255</v>
@@ -13930,16 +13903,16 @@
     </row>
     <row r="403" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B403" s="55" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C403" s="55" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="F403" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G403" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J403" s="6" t="s">
         <v>255</v>
@@ -13947,16 +13920,16 @@
     </row>
     <row r="404" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B404" s="55" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="C404" s="55" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="F404" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G404" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J404" s="6" t="s">
         <v>255</v>
@@ -13964,16 +13937,16 @@
     </row>
     <row r="405" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B405" s="55" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="C405" s="55" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="F405" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G405" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J405" s="6" t="s">
         <v>255</v>
@@ -13981,16 +13954,16 @@
     </row>
     <row r="406" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B406" s="55" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C406" s="55" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="F406" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G406" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J406" s="6" t="s">
         <v>255</v>
@@ -13998,16 +13971,16 @@
     </row>
     <row r="407" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B407" s="55" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C407" s="55" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="F407" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G407" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J407" s="6" t="s">
         <v>255</v>
@@ -14015,16 +13988,16 @@
     </row>
     <row r="408" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B408" s="55" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="C408" s="55" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="F408" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G408" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J408" s="6" t="s">
         <v>255</v>
@@ -14032,16 +14005,16 @@
     </row>
     <row r="409" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B409" s="55" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="C409" s="55" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="F409" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G409" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J409" s="6" t="s">
         <v>255</v>
@@ -14049,16 +14022,16 @@
     </row>
     <row r="410" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B410" s="55" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C410" s="55" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="F410" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G410" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J410" s="6" t="s">
         <v>255</v>
@@ -14066,16 +14039,16 @@
     </row>
     <row r="411" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B411" s="55" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="C411" s="55" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="F411" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G411" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J411" s="6" t="s">
         <v>255</v>
@@ -14083,16 +14056,16 @@
     </row>
     <row r="412" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B412" s="55" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="C412" s="55" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="F412" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G412" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J412" s="6" t="s">
         <v>255</v>
@@ -14100,16 +14073,16 @@
     </row>
     <row r="413" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B413" s="55" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="C413" s="55" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="F413" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G413" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J413" s="6" t="s">
         <v>255</v>
@@ -14117,16 +14090,16 @@
     </row>
     <row r="414" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B414" s="55" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C414" s="55" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="F414" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G414" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J414" s="6" t="s">
         <v>255</v>
@@ -14134,16 +14107,16 @@
     </row>
     <row r="415" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B415" s="55" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C415" s="55" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="F415" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G415" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J415" s="6" t="s">
         <v>255</v>
@@ -14151,16 +14124,16 @@
     </row>
     <row r="416" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B416" s="55" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="C416" s="55" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="F416" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G416" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J416" s="6" t="s">
         <v>255</v>
@@ -14168,16 +14141,16 @@
     </row>
     <row r="417" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B417" s="55" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="C417" s="55" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="F417" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G417" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J417" s="6" t="s">
         <v>255</v>
@@ -14185,16 +14158,16 @@
     </row>
     <row r="418" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B418" s="55" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C418" s="55" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="F418" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G418" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J418" s="6" t="s">
         <v>255</v>
@@ -14202,16 +14175,16 @@
     </row>
     <row r="419" spans="2:10" ht="14" x14ac:dyDescent="0.15">
       <c r="B419" s="55" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="C419" s="55" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="F419" s="3" t="s">
         <v>251</v>
       </c>
       <c r="G419" s="3" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="J419" s="6" t="s">
         <v>255</v>
@@ -14906,484 +14879,484 @@
   <sheetData>
     <row r="5" spans="6:65" x14ac:dyDescent="0.15">
       <c r="F5" s="55" t="s">
+        <v>628</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>629</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>630</v>
+      </c>
+      <c r="I5" s="55" t="s">
+        <v>631</v>
+      </c>
+      <c r="J5" s="55" t="s">
         <v>632</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="K5" s="55" t="s">
         <v>633</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="L5" s="55" t="s">
         <v>634</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="M5" s="55" t="s">
         <v>635</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="N5" s="55" t="s">
         <v>636</v>
       </c>
-      <c r="K5" s="55" t="s">
+      <c r="O5" s="55" t="s">
         <v>637</v>
       </c>
-      <c r="L5" s="55" t="s">
+      <c r="P5" s="55" t="s">
         <v>638</v>
       </c>
-      <c r="M5" s="55" t="s">
+      <c r="Q5" s="55" t="s">
         <v>639</v>
       </c>
-      <c r="N5" s="55" t="s">
+      <c r="R5" s="55" t="s">
         <v>640</v>
       </c>
-      <c r="O5" s="55" t="s">
+      <c r="S5" s="55" t="s">
         <v>641</v>
       </c>
-      <c r="P5" s="55" t="s">
+      <c r="T5" s="55" t="s">
         <v>642</v>
       </c>
-      <c r="Q5" s="55" t="s">
+      <c r="U5" s="55" t="s">
         <v>643</v>
       </c>
-      <c r="R5" s="55" t="s">
+      <c r="V5" s="55" t="s">
         <v>644</v>
       </c>
-      <c r="S5" s="55" t="s">
+      <c r="W5" s="55" t="s">
         <v>645</v>
       </c>
-      <c r="T5" s="55" t="s">
+      <c r="X5" s="55" t="s">
         <v>646</v>
       </c>
-      <c r="U5" s="55" t="s">
+      <c r="Y5" s="55" t="s">
         <v>647</v>
       </c>
-      <c r="V5" s="55" t="s">
+      <c r="Z5" s="55" t="s">
         <v>648</v>
       </c>
-      <c r="W5" s="55" t="s">
+      <c r="AA5" s="55" t="s">
         <v>649</v>
       </c>
-      <c r="X5" s="55" t="s">
+      <c r="AB5" s="55" t="s">
         <v>650</v>
       </c>
-      <c r="Y5" s="55" t="s">
+      <c r="AC5" s="55" t="s">
         <v>651</v>
       </c>
-      <c r="Z5" s="55" t="s">
+      <c r="AD5" s="55" t="s">
         <v>652</v>
       </c>
-      <c r="AA5" s="55" t="s">
+      <c r="AE5" s="55" t="s">
         <v>653</v>
       </c>
-      <c r="AB5" s="55" t="s">
+      <c r="AF5" s="55" t="s">
         <v>654</v>
       </c>
-      <c r="AC5" s="55" t="s">
+      <c r="AG5" s="55" t="s">
         <v>655</v>
       </c>
-      <c r="AD5" s="55" t="s">
+      <c r="AH5" s="55" t="s">
         <v>656</v>
       </c>
-      <c r="AE5" s="55" t="s">
+      <c r="AI5" s="55" t="s">
         <v>657</v>
       </c>
-      <c r="AF5" s="55" t="s">
+      <c r="AJ5" s="55" t="s">
         <v>658</v>
       </c>
-      <c r="AG5" s="55" t="s">
+      <c r="AK5" s="55" t="s">
         <v>659</v>
       </c>
-      <c r="AH5" s="55" t="s">
+      <c r="AL5" s="55" t="s">
         <v>660</v>
       </c>
-      <c r="AI5" s="55" t="s">
+      <c r="AM5" s="55" t="s">
         <v>661</v>
       </c>
-      <c r="AJ5" s="55" t="s">
+      <c r="AN5" s="55" t="s">
         <v>662</v>
       </c>
-      <c r="AK5" s="55" t="s">
+      <c r="AO5" s="55" t="s">
         <v>663</v>
       </c>
-      <c r="AL5" s="55" t="s">
+      <c r="AP5" s="55" t="s">
         <v>664</v>
       </c>
-      <c r="AM5" s="55" t="s">
+      <c r="AQ5" s="55" t="s">
         <v>665</v>
       </c>
-      <c r="AN5" s="55" t="s">
+      <c r="AR5" s="55" t="s">
         <v>666</v>
       </c>
-      <c r="AO5" s="55" t="s">
+      <c r="AS5" s="55" t="s">
         <v>667</v>
       </c>
-      <c r="AP5" s="55" t="s">
+      <c r="AT5" s="55" t="s">
         <v>668</v>
       </c>
-      <c r="AQ5" s="55" t="s">
+      <c r="AU5" s="55" t="s">
         <v>669</v>
       </c>
-      <c r="AR5" s="55" t="s">
+      <c r="AV5" s="55" t="s">
         <v>670</v>
       </c>
-      <c r="AS5" s="55" t="s">
+      <c r="AW5" s="55" t="s">
         <v>671</v>
       </c>
-      <c r="AT5" s="55" t="s">
+      <c r="AX5" s="55" t="s">
         <v>672</v>
       </c>
-      <c r="AU5" s="55" t="s">
+      <c r="AY5" s="55" t="s">
         <v>673</v>
       </c>
-      <c r="AV5" s="55" t="s">
+      <c r="AZ5" s="55" t="s">
         <v>674</v>
       </c>
-      <c r="AW5" s="55" t="s">
+      <c r="BA5" s="55" t="s">
         <v>675</v>
       </c>
-      <c r="AX5" s="55" t="s">
+      <c r="BB5" s="55" t="s">
         <v>676</v>
       </c>
-      <c r="AY5" s="55" t="s">
+      <c r="BC5" s="55" t="s">
         <v>677</v>
       </c>
-      <c r="AZ5" s="55" t="s">
+      <c r="BD5" s="55" t="s">
         <v>678</v>
       </c>
-      <c r="BA5" s="55" t="s">
+      <c r="BE5" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="BB5" s="55" t="s">
+      <c r="BF5" s="55" t="s">
         <v>680</v>
       </c>
-      <c r="BC5" s="55" t="s">
+      <c r="BG5" s="55" t="s">
         <v>681</v>
       </c>
-      <c r="BD5" s="55" t="s">
+      <c r="BH5" s="55" t="s">
         <v>682</v>
       </c>
-      <c r="BE5" s="55" t="s">
+      <c r="BI5" s="55" t="s">
         <v>683</v>
       </c>
-      <c r="BF5" s="55" t="s">
+      <c r="BJ5" s="55" t="s">
         <v>684</v>
       </c>
-      <c r="BG5" s="55" t="s">
+      <c r="BK5" s="55" t="s">
         <v>685</v>
       </c>
-      <c r="BH5" s="55" t="s">
+      <c r="BL5" s="55" t="s">
         <v>686</v>
       </c>
-      <c r="BI5" s="55" t="s">
+      <c r="BM5" s="55" t="s">
         <v>687</v>
-      </c>
-      <c r="BJ5" s="55" t="s">
-        <v>688</v>
-      </c>
-      <c r="BK5" s="55" t="s">
-        <v>689</v>
-      </c>
-      <c r="BL5" s="55" t="s">
-        <v>690</v>
-      </c>
-      <c r="BM5" s="55" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="7" spans="6:65" x14ac:dyDescent="0.15">
       <c r="F7" s="55" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="8" spans="6:65" x14ac:dyDescent="0.15">
       <c r="F8" s="55" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="9" spans="6:65" x14ac:dyDescent="0.15">
       <c r="F9" s="55" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="10" spans="6:65" x14ac:dyDescent="0.15">
       <c r="F10" s="55" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
     </row>
     <row r="11" spans="6:65" x14ac:dyDescent="0.15">
       <c r="F11" s="55" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="12" spans="6:65" x14ac:dyDescent="0.15">
       <c r="F12" s="55" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="13" spans="6:65" x14ac:dyDescent="0.15">
       <c r="F13" s="55" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="14" spans="6:65" x14ac:dyDescent="0.15">
       <c r="F14" s="55" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="15" spans="6:65" x14ac:dyDescent="0.15">
       <c r="F15" s="55" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
     </row>
     <row r="16" spans="6:65" x14ac:dyDescent="0.15">
       <c r="F16" s="55" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F17" s="55" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F18" s="55" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F19" s="55" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F20" s="55" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F21" s="55" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F22" s="55" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F23" s="55" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F24" s="55" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F25" s="55" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F26" s="55" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F27" s="55" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F28" s="55" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F29" s="55" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
     </row>
     <row r="30" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F30" s="55" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
     </row>
     <row r="31" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F31" s="55" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="32" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F32" s="55" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F33" s="55" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F34" s="55" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F35" s="55" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="36" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F36" s="55" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="37" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F37" s="55" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
     </row>
     <row r="38" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F38" s="55" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
     </row>
     <row r="39" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F39" s="55" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
     </row>
     <row r="40" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F40" s="55" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="41" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F41" s="55" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
     </row>
     <row r="42" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F42" s="55" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
     </row>
     <row r="43" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F43" s="55" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="44" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F44" s="55" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="45" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F45" s="55" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
     </row>
     <row r="46" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F46" s="55" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
     </row>
     <row r="47" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F47" s="55" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="48" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F48" s="55" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="49" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F49" s="55" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="50" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F50" s="55" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
     </row>
     <row r="51" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F51" s="55" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="52" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F52" s="55" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="53" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F53" s="55" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="54" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F54" s="55" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="55" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F55" s="55" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="56" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F56" s="55" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="57" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F57" s="55" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
     </row>
     <row r="58" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F58" s="55" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
     </row>
     <row r="59" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F59" s="55" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="60" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F60" s="55" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="61" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F61" s="55" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
     </row>
     <row r="62" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F62" s="55" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="63" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F63" s="55" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="64" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F64" s="55" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
     </row>
     <row r="65" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F65" s="55" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
     </row>
     <row r="66" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F66" s="55" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>